<commit_message>
Changes associated with removing unknown as a permitted spreadsheet value
</commit_message>
<xml_diff>
--- a/metadata/juno/metadata/tests/test-data-files/valid_spreadsheet.xlsx
+++ b/metadata/juno/metadata/tests/test-data-files/valid_spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kp11/workspace/pathogens-gitlab/monocle/metadata/juno/metadata/tests/test-data-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110E9E3A-7CFE-F444-AAE1-03F211498E7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08CD9A6-928D-6B41-92C0-CDE75EB68543}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="4220" windowWidth="31100" windowHeight="10500" xr2:uid="{C6880AE4-86A7-2445-AC81-7EA4C295E861}"/>
+    <workbookView xWindow="1360" yWindow="4220" windowWidth="32980" windowHeight="14480" xr2:uid="{C6880AE4-86A7-2445-AC81-7EA4C295E861}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="207">
   <si>
     <t>Country</t>
   </si>
@@ -524,6 +524,241 @@
       </rPr>
       <t>human, bovine, fish, camel, other (enter species name if known)</t>
     </r>
+  </si>
+  <si>
+    <t>For options please refer to 'Entry values' tab; if carriage sample, please enter 'NA'</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sample isolation source/site; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>for options please refer to 'Entry values' tab</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Options: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ia, Ib, II, III, IV, V, VI, VII, VIII, IX, NT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For maternal carriage isolates only; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>for Options please refer to 'Entry values' tab</t>
+    </r>
+  </si>
+  <si>
+    <t>For maternal carriage or neonatal carriage/disease isolates only</t>
+  </si>
+  <si>
+    <t>Lane_ID</t>
+  </si>
+  <si>
+    <t>adult</t>
+  </si>
+  <si>
+    <t>invasive disease</t>
+  </si>
+  <si>
+    <r>
+      <t>Was isolate selected randomly?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Options: yes/no</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Options: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>disk diffusion; broth dilution; agar dilution; Etest</t>
+    </r>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>1000STDY7000167</t>
+  </si>
+  <si>
+    <t>1000STDY7000168</t>
+  </si>
+  <si>
+    <t>1000STDY7000169</t>
+  </si>
+  <si>
+    <t>50000_2#282</t>
+  </si>
+  <si>
+    <t>50000_2#287</t>
+  </si>
+  <si>
+    <t>50000_2#291</t>
+  </si>
+  <si>
+    <t>50000_2#296</t>
+  </si>
+  <si>
+    <t>Test Institution A</t>
+  </si>
+  <si>
+    <t>TestCountryA</t>
+  </si>
+  <si>
+    <t>EY70425</t>
+  </si>
+  <si>
+    <t>EY_70602</t>
+  </si>
+  <si>
+    <t>PMID: 12345678</t>
+  </si>
+  <si>
+    <t>PMID: 1234567, PMID: 12345678</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>infant</t>
+  </si>
+  <si>
+    <t>Adolescent</t>
+  </si>
+  <si>
+    <t>Lancefield</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Etest</t>
+  </si>
+  <si>
+    <t>agar dilution</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>disk diffusion</t>
+  </si>
+  <si>
+    <t>1000STDY7000166</t>
+  </si>
+  <si>
+    <t>EY_70601</t>
+  </si>
+  <si>
+    <t>EY70603</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Invasive disease</t>
+  </si>
+  <si>
+    <t>Bacteraemia</t>
+  </si>
+  <si>
+    <t>Blood</t>
+  </si>
+  <si>
+    <t>Latex AGGLUTINATION</t>
+  </si>
+  <si>
+    <t>Arthritis</t>
+  </si>
+  <si>
+    <t>Human</t>
+  </si>
+  <si>
+    <t>Neonate</t>
+  </si>
+  <si>
+    <t>Carriage</t>
+  </si>
+  <si>
+    <t>Other sterile site</t>
+  </si>
+  <si>
+    <t>CD_XX_EW00001</t>
+  </si>
+  <si>
+    <t>CD_XX_EW00002</t>
+  </si>
+  <si>
+    <t>CD_XX_EW00003</t>
+  </si>
+  <si>
+    <t>CD_XX_EW00004</t>
+  </si>
+  <si>
+    <t>TEST-stUDY NA_ME1 (123), [ABC] %.</t>
   </si>
   <si>
     <r>
@@ -543,7 +778,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>: neonate, infant, child, adolescent, adult, unknown. For reference please check the 'Age classification' tab</t>
+      <t>: neonate, infant, child, adolescent, adult. For reference please check the 'Age classification' tab</t>
     </r>
   </si>
   <si>
@@ -564,11 +799,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>: carriage, invasive disease, non-invasive disease, unknown</t>
-    </r>
-  </si>
-  <si>
-    <t>For options please refer to 'Entry values' tab; if carriage sample, please enter 'NA'</t>
+      <t>: carriage, invasive disease, non-invasive disease</t>
+    </r>
   </si>
   <si>
     <r>
@@ -588,12 +820,12 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>EOD, LOD, VLOD, unknown; If other disease or carriage please enter 'NA'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Sample isolation source/site; </t>
+      <t>EOD, LOD, VLOD; If other disease or carriage please enter 'NA'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>For maternal carriage isolates only; Options:</t>
     </r>
     <r>
       <rPr>
@@ -602,243 +834,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>for options please refer to 'Entry values' tab</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Options: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ia, Ib, II, III, IV, V, VI, VII, VIII, IX, NT</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">For maternal carriage isolates only; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>for Options please refer to 'Entry values' tab</t>
-    </r>
-  </si>
-  <si>
-    <t>For maternal carriage or neonatal carriage/disease isolates only</t>
-  </si>
-  <si>
-    <t>Lane_ID</t>
-  </si>
-  <si>
-    <t>adult</t>
-  </si>
-  <si>
-    <t>invasive disease</t>
-  </si>
-  <si>
-    <r>
-      <t>Was isolate selected randomly?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Options: yes/no</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>For maternal carriage isolates only; Options:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> yes, no, unknown</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Options: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>disk diffusion; broth dilution; agar dilution; Etest</t>
-    </r>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>VI</t>
-  </si>
-  <si>
-    <t>III</t>
-  </si>
-  <si>
-    <t>1000STDY7000167</t>
-  </si>
-  <si>
-    <t>1000STDY7000168</t>
-  </si>
-  <si>
-    <t>1000STDY7000169</t>
-  </si>
-  <si>
-    <t>50000_2#282</t>
-  </si>
-  <si>
-    <t>50000_2#287</t>
-  </si>
-  <si>
-    <t>50000_2#291</t>
-  </si>
-  <si>
-    <t>50000_2#296</t>
-  </si>
-  <si>
-    <t>Test Institution A</t>
-  </si>
-  <si>
-    <t>TestCountryA</t>
-  </si>
-  <si>
-    <t>EY70425</t>
-  </si>
-  <si>
-    <t>EY_70602</t>
-  </si>
-  <si>
-    <t>PMID: 12345678</t>
-  </si>
-  <si>
-    <t>PMID: 1234567, PMID: 12345678</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>London</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>infant</t>
-  </si>
-  <si>
-    <t>Adolescent</t>
-  </si>
-  <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>Lancefield</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>Etest</t>
-  </si>
-  <si>
-    <t>agar dilution</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>disk diffusion</t>
-  </si>
-  <si>
-    <t>1000STDY7000166</t>
-  </si>
-  <si>
-    <t>EY_70601</t>
-  </si>
-  <si>
-    <t>EY70603</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>Invasive disease</t>
-  </si>
-  <si>
-    <t>Bacteraemia</t>
-  </si>
-  <si>
-    <t>Blood</t>
-  </si>
-  <si>
-    <t>Latex AGGLUTINATION</t>
-  </si>
-  <si>
-    <t>Arthritis</t>
-  </si>
-  <si>
-    <t>Human</t>
-  </si>
-  <si>
-    <t>Neonate</t>
-  </si>
-  <si>
-    <t>Carriage</t>
-  </si>
-  <si>
-    <t>Other sterile site</t>
-  </si>
-  <si>
-    <t>CD_XX_EW00001</t>
-  </si>
-  <si>
-    <t>CD_XX_EW00002</t>
-  </si>
-  <si>
-    <t>CD_XX_EW00003</t>
-  </si>
-  <si>
-    <t>CD_XX_EW00004</t>
-  </si>
-  <si>
-    <t>TEST-stUDY NA_ME1 (123), [ABC] %.</t>
+      <t xml:space="preserve"> yes, no</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1373,10 +1370,10 @@
   <dimension ref="A1:BI7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="R4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1604,7 +1601,7 @@
         <v>84</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>82</v>
@@ -1634,7 +1631,7 @@
         <v>98</v>
       </c>
       <c r="Q2" s="10" t="s">
-        <v>143</v>
+        <v>203</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>90</v>
@@ -1649,121 +1646,121 @@
         <v>92</v>
       </c>
       <c r="V2" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="X2" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="Y2" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="W2" s="11" t="s">
+      <c r="Z2" s="8" t="s">
         <v>145</v>
-      </c>
-      <c r="X2" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="Y2" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="Z2" s="8" t="s">
-        <v>148</v>
       </c>
       <c r="AA2" s="8" t="s">
         <v>96</v>
       </c>
       <c r="AB2" s="12" t="s">
-        <v>155</v>
+        <v>206</v>
       </c>
       <c r="AC2" s="12" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="AD2" s="12" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="AE2" s="12" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="AF2" s="12" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="AG2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="AH2" s="23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="AI2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="AJ2" s="23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="AK2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="AL2" s="23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="AM2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="AN2" s="23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="AO2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="AP2" s="23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="AQ2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="AR2" s="23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="AS2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="AT2" s="23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="AU2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="AV2" s="23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="AW2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="AX2" s="23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="AY2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="AZ2" s="23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="BA2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="BB2" s="23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="BC2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="BD2" s="23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="BE2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="BF2" s="23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="BG2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="BH2" s="23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="BI2" s="6" t="s">
         <v>97</v>
@@ -1780,7 +1777,7 @@
         <v>105</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>106</v>
@@ -1953,37 +1950,37 @@
     </row>
     <row r="4" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C4" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F4" t="s">
+        <v>169</v>
+      </c>
+      <c r="G4" t="s">
+        <v>187</v>
+      </c>
+      <c r="H4" t="s">
+        <v>165</v>
+      </c>
+      <c r="I4" t="s">
+        <v>172</v>
+      </c>
+      <c r="J4" t="s">
+        <v>171</v>
+      </c>
+      <c r="K4" t="s">
         <v>164</v>
-      </c>
-      <c r="E4" t="s">
-        <v>207</v>
-      </c>
-      <c r="F4" t="s">
-        <v>173</v>
-      </c>
-      <c r="G4" t="s">
-        <v>192</v>
-      </c>
-      <c r="H4" t="s">
-        <v>169</v>
-      </c>
-      <c r="I4" t="s">
-        <v>176</v>
-      </c>
-      <c r="J4" t="s">
-        <v>175</v>
-      </c>
-      <c r="K4" t="s">
-        <v>168</v>
       </c>
       <c r="L4">
         <v>2014</v>
@@ -1995,16 +1992,13 @@
         <v>2</v>
       </c>
       <c r="O4" t="s">
-        <v>199</v>
-      </c>
-      <c r="P4" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="Q4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="V4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="W4" t="s">
         <v>35</v>
@@ -2016,16 +2010,16 @@
         <v>25</v>
       </c>
       <c r="Z4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="AA4" t="s">
         <v>137</v>
       </c>
       <c r="AB4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="AC4" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="AD4">
         <v>12</v>
@@ -2040,111 +2034,111 @@
         <v>1.2</v>
       </c>
       <c r="AH4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="AI4">
         <v>10.334545</v>
       </c>
       <c r="AJ4" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="AK4">
         <v>100.4</v>
       </c>
       <c r="AL4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="AM4">
         <v>1000.5</v>
       </c>
       <c r="AN4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="AO4">
         <v>10000.6</v>
       </c>
       <c r="AP4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="AQ4">
         <v>100000.7</v>
       </c>
       <c r="AR4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="AS4">
         <v>20.8</v>
       </c>
       <c r="AT4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="AU4">
         <v>70.400000000000006</v>
       </c>
       <c r="AV4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="AW4">
         <v>0.3</v>
       </c>
       <c r="AX4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="AY4">
         <v>12.2</v>
       </c>
       <c r="AZ4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="BA4">
         <v>10.1</v>
       </c>
       <c r="BB4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="BC4">
         <v>10</v>
       </c>
       <c r="BD4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="BE4">
         <v>100</v>
       </c>
       <c r="BF4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="BG4">
         <v>20</v>
       </c>
       <c r="BH4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5" t="s">
         <v>161</v>
       </c>
-      <c r="B5" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="C5" t="s">
-        <v>204</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G5" t="s">
+        <v>188</v>
+      </c>
+      <c r="H5" t="s">
         <v>165</v>
       </c>
-      <c r="F5" t="s">
-        <v>172</v>
-      </c>
-      <c r="G5" t="s">
-        <v>193</v>
-      </c>
-      <c r="H5" t="s">
-        <v>169</v>
-      </c>
       <c r="K5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="L5">
         <v>2014</v>
@@ -2152,142 +2146,118 @@
       <c r="O5" t="s">
         <v>136</v>
       </c>
-      <c r="P5" t="s">
-        <v>71</v>
-      </c>
       <c r="Q5" t="s">
-        <v>152</v>
+        <v>149</v>
+      </c>
+      <c r="R5">
+        <v>25</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>2</v>
       </c>
       <c r="V5" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="W5" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="X5" t="s">
         <v>72</v>
       </c>
       <c r="Y5" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="Z5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="AA5" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="AB5" t="s">
-        <v>193</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>181</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>181</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>181</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="AG5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="AI5" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="AK5" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="AM5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="AO5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="AQ5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="AS5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="AU5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="AW5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="AY5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="BA5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="BC5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="BE5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="BG5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D6" t="s">
         <v>162</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="C6" t="s">
-        <v>205</v>
-      </c>
-      <c r="D6" t="s">
-        <v>166</v>
-      </c>
       <c r="G6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H6" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="K6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="L6">
         <v>2014</v>
       </c>
-      <c r="M6" t="s">
-        <v>181</v>
-      </c>
-      <c r="N6" t="s">
-        <v>181</v>
-      </c>
-      <c r="O6" t="s">
-        <v>181</v>
-      </c>
       <c r="P6" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="Q6" t="s">
-        <v>179</v>
-      </c>
-      <c r="R6" t="s">
-        <v>181</v>
-      </c>
-      <c r="S6" t="s">
-        <v>181</v>
-      </c>
-      <c r="T6" t="s">
-        <v>181</v>
-      </c>
-      <c r="U6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="V6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="W6" t="s">
         <v>64</v>
@@ -2299,36 +2269,30 @@
         <v>25</v>
       </c>
       <c r="Z6" t="s">
-        <v>160</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>181</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="C7" t="s">
+        <v>201</v>
+      </c>
+      <c r="D7" t="s">
         <v>163</v>
       </c>
-      <c r="B7" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="C7" t="s">
-        <v>206</v>
-      </c>
-      <c r="D7" t="s">
-        <v>167</v>
-      </c>
       <c r="G7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H7" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="K7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="L7">
         <v>2014</v>
@@ -2337,13 +2301,25 @@
         <v>136</v>
       </c>
       <c r="P7" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="Q7" t="s">
-        <v>180</v>
+        <v>176</v>
+      </c>
+      <c r="R7">
+        <v>15</v>
+      </c>
+      <c r="S7">
+        <v>10</v>
+      </c>
+      <c r="T7">
+        <v>2</v>
+      </c>
+      <c r="U7">
+        <v>4</v>
       </c>
       <c r="V7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="W7" t="s">
         <v>72</v>
@@ -2352,13 +2328,13 @@
         <v>72</v>
       </c>
       <c r="Y7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="Z7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AA7" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix for enforcing consistent upload spreadsheet value casing
</commit_message>
<xml_diff>
--- a/metadata/juno/metadata/tests/test-data-files/valid_spreadsheet.xlsx
+++ b/metadata/juno/metadata/tests/test-data-files/valid_spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kp11/workspace/pathogens-gitlab/monocle/metadata/juno/metadata/tests/test-data-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08CD9A6-928D-6B41-92C0-CDE75EB68543}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55BE194-75A2-8344-81AD-3B05ECF42827}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="4220" windowWidth="32980" windowHeight="14480" xr2:uid="{C6880AE4-86A7-2445-AC81-7EA4C295E861}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="209">
   <si>
     <t>Country</t>
   </si>
@@ -497,9 +497,6 @@
     <t>human</t>
   </si>
   <si>
-    <t>PCR</t>
-  </si>
-  <si>
     <t>EOD</t>
   </si>
   <si>
@@ -683,9 +680,6 @@
     <t>Adolescent</t>
   </si>
   <si>
-    <t>Lancefield</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
@@ -726,9 +720,6 @@
   </si>
   <si>
     <t>Blood</t>
-  </si>
-  <si>
-    <t>Latex AGGLUTINATION</t>
   </si>
   <si>
     <t>Arthritis</t>
@@ -836,6 +827,21 @@
       </rPr>
       <t xml:space="preserve"> yes, no</t>
     </r>
+  </si>
+  <si>
+    <t>Latex AGGLUTINATION, PCR</t>
+  </si>
+  <si>
+    <t>pcr</t>
+  </si>
+  <si>
+    <t>lancefield</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>etest</t>
   </si>
 </sst>
 </file>
@@ -1370,10 +1376,10 @@
   <dimension ref="A1:BI7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="R4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="AD4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W7" sqref="W7"/>
+      <selection pane="bottomRight" activeCell="AI16" sqref="AI16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1387,7 +1393,8 @@
     <col min="11" max="11" width="33.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="23" width="17.83203125" customWidth="1"/>
     <col min="24" max="24" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="17.83203125" customWidth="1"/>
+    <col min="25" max="26" width="17.83203125" customWidth="1"/>
+    <col min="27" max="27" width="51.5" customWidth="1"/>
     <col min="28" max="28" width="27" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="24.33203125" bestFit="1" customWidth="1"/>
@@ -1583,13 +1590,13 @@
     </row>
     <row r="2" spans="1:61" ht="150" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>133</v>
@@ -1601,7 +1608,7 @@
         <v>84</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>82</v>
@@ -1625,13 +1632,13 @@
         <v>87</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>98</v>
       </c>
       <c r="Q2" s="10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>90</v>
@@ -1646,121 +1653,121 @@
         <v>92</v>
       </c>
       <c r="V2" s="11" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="W2" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="X2" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y2" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="X2" s="22" t="s">
-        <v>205</v>
-      </c>
-      <c r="Y2" s="9" t="s">
+      <c r="Z2" s="8" t="s">
         <v>144</v>
-      </c>
-      <c r="Z2" s="8" t="s">
-        <v>145</v>
       </c>
       <c r="AA2" s="8" t="s">
         <v>96</v>
       </c>
       <c r="AB2" s="12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AC2" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="AD2" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="AD2" s="12" t="s">
-        <v>147</v>
-      </c>
       <c r="AE2" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AF2" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AG2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="AH2" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AI2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="AJ2" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AK2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="AL2" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AM2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="AN2" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AO2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="AP2" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AQ2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="AR2" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AS2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="AT2" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AU2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="AV2" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AW2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="AX2" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AY2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="AZ2" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="BA2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="BB2" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="BC2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="BD2" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="BE2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="BF2" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="BG2" s="23" t="s">
         <v>2</v>
       </c>
       <c r="BH2" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="BI2" s="6" t="s">
         <v>97</v>
@@ -1777,7 +1784,7 @@
         <v>105</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>106</v>
@@ -1950,37 +1957,37 @@
     </row>
     <row r="4" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L4">
         <v>2014</v>
@@ -1992,34 +1999,37 @@
         <v>2</v>
       </c>
       <c r="O4" t="s">
-        <v>194</v>
+        <v>191</v>
+      </c>
+      <c r="P4" t="s">
+        <v>207</v>
       </c>
       <c r="Q4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="V4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="W4" t="s">
         <v>35</v>
       </c>
       <c r="X4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Y4" t="s">
         <v>25</v>
       </c>
       <c r="Z4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AA4" t="s">
-        <v>137</v>
+        <v>205</v>
       </c>
       <c r="AB4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AC4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="AD4">
         <v>12</v>
@@ -2034,111 +2044,111 @@
         <v>1.2</v>
       </c>
       <c r="AH4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="AI4">
         <v>10.334545</v>
       </c>
       <c r="AJ4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="AK4">
         <v>100.4</v>
       </c>
       <c r="AL4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AM4">
         <v>1000.5</v>
       </c>
       <c r="AN4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AO4">
         <v>10000.6</v>
       </c>
       <c r="AP4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AQ4">
         <v>100000.7</v>
       </c>
       <c r="AR4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AS4">
         <v>20.8</v>
       </c>
       <c r="AT4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AU4">
         <v>70.400000000000006</v>
       </c>
       <c r="AV4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AW4">
         <v>0.3</v>
       </c>
       <c r="AX4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AY4">
         <v>12.2</v>
       </c>
       <c r="AZ4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="BA4">
         <v>10.1</v>
       </c>
       <c r="BB4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="BC4">
         <v>10</v>
       </c>
       <c r="BD4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="BE4">
         <v>100</v>
       </c>
       <c r="BF4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="BG4">
         <v>20</v>
       </c>
       <c r="BH4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L5">
         <v>2014</v>
@@ -2147,7 +2157,7 @@
         <v>136</v>
       </c>
       <c r="Q5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="R5">
         <v>25</v>
@@ -2162,137 +2172,143 @@
         <v>2</v>
       </c>
       <c r="V5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="W5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="X5" t="s">
         <v>72</v>
       </c>
       <c r="Y5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="Z5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AA5" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="AB5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AG5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AI5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AK5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="AM5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AO5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AQ5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AS5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AU5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AW5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AY5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BA5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BC5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BE5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="BG5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L6">
         <v>2014</v>
       </c>
       <c r="P6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Q6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="V6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="W6" t="s">
         <v>64</v>
       </c>
       <c r="X6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Y6" t="s">
         <v>25</v>
       </c>
       <c r="Z6" t="s">
-        <v>156</v>
+        <v>155</v>
+      </c>
+      <c r="AG6">
+        <v>1</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
+        <v>162</v>
+      </c>
+      <c r="G7" t="s">
+        <v>152</v>
+      </c>
+      <c r="H7" t="s">
+        <v>164</v>
+      </c>
+      <c r="K7" t="s">
         <v>163</v>
-      </c>
-      <c r="G7" t="s">
-        <v>153</v>
-      </c>
-      <c r="H7" t="s">
-        <v>165</v>
-      </c>
-      <c r="K7" t="s">
-        <v>164</v>
       </c>
       <c r="L7">
         <v>2014</v>
@@ -2301,10 +2317,10 @@
         <v>136</v>
       </c>
       <c r="P7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="Q7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="R7">
         <v>15</v>
@@ -2319,7 +2335,7 @@
         <v>4</v>
       </c>
       <c r="V7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="W7" t="s">
         <v>72</v>
@@ -2328,13 +2344,13 @@
         <v>72</v>
       </c>
       <c r="Y7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="Z7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AA7" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>